<commit_message>
rewite code to modelize
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="108">
   <si>
     <t>kNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -361,6 +360,94 @@
   </si>
   <si>
     <t>oripca_new(rf.adb)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_cos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_sin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_tan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arccos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arcsin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arctan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_arccos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_arcsin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_arctan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>square</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_squre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>norma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_nomar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pca</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_pca</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_newly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newlyxy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori_newlyxy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4751,10 +4838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:AM50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5357,7 +5444,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
@@ -5385,8 +5472,74 @@
       <c r="L17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" t="s">
+        <v>86</v>
+      </c>
+      <c r="S17" t="s">
+        <v>87</v>
+      </c>
+      <c r="T17" t="s">
+        <v>88</v>
+      </c>
+      <c r="U17" t="s">
+        <v>89</v>
+      </c>
+      <c r="V17" t="s">
+        <v>90</v>
+      </c>
+      <c r="W17" t="s">
+        <v>91</v>
+      </c>
+      <c r="X17" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -5419,7 +5572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -5452,7 +5605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -5485,7 +5638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -5518,7 +5671,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -5551,7 +5704,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -5584,7 +5737,7 @@
         <v>98.909090909090907</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -5617,7 +5770,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -5650,7 +5803,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <f>SUM(B18:B25)</f>
         <v>797.09999999999991</v>
@@ -5675,14 +5828,17 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q26" s="4">
+        <f>SUM(Q18:Q25)</f>
+        <v>798.90909090909088</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
@@ -5711,7 +5867,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -5756,7 +5912,7 @@
         <v>86.764705882352899</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -5801,7 +5957,7 @@
         <v>86.764705882352899</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>